<commit_message>
finished steps for whitesource
</commit_message>
<xml_diff>
--- a/Packaged Sprint/PackagedSprint.xlsx
+++ b/Packaged Sprint/PackagedSprint.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11113"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10106"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/richardguthrie/git_repos/DevOps_DevSecOps/Packaged Sprint/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/doyleturner/Projects/DevOps_DevSecOps/Packaged Sprint/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{30AA8474-2505-C348-9DF6-5C16016D8F18}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5829691B-9A00-6144-9CFC-87F0A1BC950F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F88568D6-CCC9-B049-A3B6-7C0DD299A0A6}"/>
+    <workbookView xWindow="51200" yWindow="0" windowWidth="51200" windowHeight="28800" xr2:uid="{F88568D6-CCC9-B049-A3B6-7C0DD299A0A6}"/>
   </bookViews>
   <sheets>
     <sheet name="PackagedSprint_Export" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
   <si>
     <t>User Story</t>
   </si>
@@ -117,6 +117,60 @@
   </si>
   <si>
     <t>Enable Quality Gates</t>
+  </si>
+  <si>
+    <t>Dependency and Container Scanning</t>
+  </si>
+  <si>
+    <t>ryan.harrington@whitesourcesoftware.com</t>
+  </si>
+  <si>
+    <t>Have an admin user created</t>
+  </si>
+  <si>
+    <t>Add User</t>
+  </si>
+  <si>
+    <t>Add User to Admin Group</t>
+  </si>
+  <si>
+    <t>Create a "Product" in WS</t>
+  </si>
+  <si>
+    <t>Create Product</t>
+  </si>
+  <si>
+    <t>Create "Project(s)" under the Product</t>
+  </si>
+  <si>
+    <t>Link WS &amp; AzDO</t>
+  </si>
+  <si>
+    <t>Connect WS to AzDO</t>
+  </si>
+  <si>
+    <t>WhiteSource Code Dependency Scanning</t>
+  </si>
+  <si>
+    <t>Request or Have Customer Request WhiteSource Account</t>
+  </si>
+  <si>
+    <t>Create Project(s)</t>
+  </si>
+  <si>
+    <t>Add WS Configuration to Source</t>
+  </si>
+  <si>
+    <t>Add Configuration</t>
+  </si>
+  <si>
+    <t>Configure Azure DevOps for WhiteSource</t>
+  </si>
+  <si>
+    <t>Azure Devops Tasks</t>
+  </si>
+  <si>
+    <t>WhiteSource ADO Template</t>
   </si>
 </sst>
 </file>
@@ -501,17 +555,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56AC572D-7177-9C48-AF1B-1F88119811DE}">
-  <dimension ref="A1:D18"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:D35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="50.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="90.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -602,36 +657,112 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D16" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C17" t="s">
+        <v>33</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C18" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C19" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C20" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="C21" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B30" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B14" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B31" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B15" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="C16" t="s">
+    <row r="33" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C17" t="s">
+    <row r="34" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C34" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C18" t="s">
+    <row r="35" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C35" t="s">
         <v>27</v>
       </c>
     </row>
@@ -644,11 +775,20 @@
     <hyperlink ref="D8" r:id="rId5" xr:uid="{D6ECCFEC-099D-BF42-82DC-FCC59D756EFE}"/>
     <hyperlink ref="D10" r:id="rId6" xr:uid="{D6F47483-0B7D-F34C-9576-2AE66E48B3CF}"/>
     <hyperlink ref="D11" r:id="rId7" xr:uid="{03395D31-3A4E-BC4D-8D0F-0FFF8F4D9558}"/>
+    <hyperlink ref="D14" r:id="rId8" display="mailto:ryan.harrington@whitesourcesoftware.com" xr:uid="{2701EFF9-0C9F-614D-A963-E51474669718}"/>
+    <hyperlink ref="D15" r:id="rId9" location="add-users" xr:uid="{3F24DF7F-B3A8-6C49-B421-50FCBEA5B1E1}"/>
+    <hyperlink ref="D16" r:id="rId10" location="add-users-to-admin-group" xr:uid="{93E7333B-EA2F-AE46-BD2A-6F5D535E859A}"/>
+    <hyperlink ref="D17" r:id="rId11" location="add-product" xr:uid="{AC49FEB6-486E-0145-A844-B6911F10286D}"/>
+    <hyperlink ref="D19" r:id="rId12" location="shorten-the-feedback-loop--connect-azure-devops-to-whitesource" xr:uid="{114FCF25-27AB-C749-88C5-11F96F2634FA}"/>
+    <hyperlink ref="D18" r:id="rId13" location="add-projects" xr:uid="{56A947D0-1A1A-8E47-AF1E-EE11E5FA46EC}"/>
+    <hyperlink ref="D20" r:id="rId14" location="add-whitesource-configuration-to-source-code" xr:uid="{4D15333A-3BFD-7F49-ADB4-92C03AB5B83A}"/>
+    <hyperlink ref="D21" r:id="rId15" location="configure-azure-devops" xr:uid="{7750A669-BFFC-224E-841D-B1B7D41DBFE5}"/>
+    <hyperlink ref="D22" r:id="rId16" xr:uid="{0708A982-067B-FB44-8514-B5D4FB1B14AB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <tableParts count="1">
-    <tablePart r:id="rId8"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>